<commit_message>
remove trait from list if played as often as present in deck
</commit_message>
<xml_diff>
--- a/DoomPy/cards.xlsx
+++ b/DoomPy/cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azabicki/Sync/Projects/Doomlings/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azabicki/Sync/Projects/DoomPy/DoomPy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA09DF10-B379-0347-8850-35ABC7ECDD46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863DC743-7687-BA45-8864-66DAAA38FEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15320" activeTab="1" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15320" xr2:uid="{FFCA0E03-569E-F44B-8E00-2A40D4903513}"/>
   </bookViews>
   <sheets>
     <sheet name="traits" sheetId="1" r:id="rId1"/>
@@ -868,7 +868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -891,7 +891,6 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1215,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AE435C-BBFF-4D4C-B457-AFC1FAEE6491}">
   <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G121" sqref="G121:G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1271,7 +1270,9 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2"/>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1292,7 +1293,9 @@
       <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="G3"/>
+      <c r="G3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1313,7 +1316,9 @@
       <c r="F4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G4"/>
+      <c r="G4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1332,7 +1337,9 @@
         <v>9</v>
       </c>
       <c r="F5"/>
-      <c r="G5"/>
+      <c r="G5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1351,7 +1358,9 @@
         <v>226</v>
       </c>
       <c r="F6"/>
-      <c r="G6"/>
+      <c r="G6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1370,7 +1379,9 @@
         <v>12</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7"/>
+      <c r="G7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1389,7 +1400,9 @@
         <v>9</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8"/>
+      <c r="G8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1408,7 +1421,9 @@
         <v>9</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9"/>
+      <c r="G9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1427,7 +1442,9 @@
         <v>227</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10"/>
+      <c r="G10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1446,7 +1463,9 @@
         <v>9</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11"/>
+      <c r="G11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1465,7 +1484,9 @@
         <v>226</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12"/>
+      <c r="G12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1484,7 +1505,9 @@
         <v>9</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="G13"/>
+      <c r="G13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1503,7 +1526,9 @@
         <v>226</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14"/>
+      <c r="G14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1522,7 +1547,9 @@
         <v>9</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15"/>
+      <c r="G15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1541,7 +1568,9 @@
         <v>1</v>
       </c>
       <c r="F16" s="3"/>
-      <c r="G16"/>
+      <c r="G16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1560,7 +1589,9 @@
         <v>1</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17"/>
+      <c r="G17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1579,7 +1610,9 @@
         <v>9</v>
       </c>
       <c r="F18" s="3"/>
-      <c r="G18"/>
+      <c r="G18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1598,7 +1631,9 @@
         <v>226</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19"/>
+      <c r="G19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1617,7 +1652,9 @@
         <v>9</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20"/>
+      <c r="G20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1636,7 +1673,9 @@
         <v>9</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21"/>
+      <c r="G21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1655,7 +1694,9 @@
         <v>9</v>
       </c>
       <c r="F22" s="3"/>
-      <c r="G22"/>
+      <c r="G22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -1674,7 +1715,9 @@
         <v>9</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23"/>
+      <c r="G23">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1695,7 +1738,9 @@
       <c r="F24" t="s">
         <v>3</v>
       </c>
-      <c r="G24"/>
+      <c r="G24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1716,7 +1761,9 @@
       <c r="F25" t="s">
         <v>3</v>
       </c>
-      <c r="G25"/>
+      <c r="G25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1737,7 +1784,9 @@
       <c r="F26" t="s">
         <v>3</v>
       </c>
-      <c r="G26"/>
+      <c r="G26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -1756,7 +1805,9 @@
         <v>226</v>
       </c>
       <c r="F27"/>
-      <c r="G27"/>
+      <c r="G27">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -1775,7 +1826,9 @@
         <v>226</v>
       </c>
       <c r="F28"/>
-      <c r="G28"/>
+      <c r="G28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1794,7 +1847,9 @@
         <v>227</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="G29"/>
+      <c r="G29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1813,7 +1868,9 @@
         <v>226</v>
       </c>
       <c r="F30" s="3"/>
-      <c r="G30"/>
+      <c r="G30">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1832,7 +1889,9 @@
         <v>1</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31"/>
+      <c r="G31">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1851,7 +1910,9 @@
         <v>227</v>
       </c>
       <c r="F32" s="3"/>
-      <c r="G32"/>
+      <c r="G32">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -1870,7 +1931,9 @@
         <v>226</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33"/>
+      <c r="G33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1889,7 +1952,9 @@
         <v>227</v>
       </c>
       <c r="F34" s="3"/>
-      <c r="G34"/>
+      <c r="G34">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1908,7 +1973,9 @@
         <v>9</v>
       </c>
       <c r="F35"/>
-      <c r="G35"/>
+      <c r="G35">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1927,7 +1994,9 @@
         <v>227</v>
       </c>
       <c r="F36" s="3"/>
-      <c r="G36"/>
+      <c r="G36">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1946,7 +2015,9 @@
         <v>9</v>
       </c>
       <c r="F37"/>
-      <c r="G37"/>
+      <c r="G37">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -1965,7 +2036,9 @@
         <v>227</v>
       </c>
       <c r="F38" s="3"/>
-      <c r="G38"/>
+      <c r="G38">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -1984,7 +2057,9 @@
         <v>9</v>
       </c>
       <c r="F39"/>
-      <c r="G39"/>
+      <c r="G39">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -2024,7 +2099,9 @@
         <v>9</v>
       </c>
       <c r="F41"/>
-      <c r="G41"/>
+      <c r="G41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -2043,7 +2120,9 @@
         <v>9</v>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42"/>
+      <c r="G42">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -2062,7 +2141,9 @@
         <v>226</v>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43"/>
+      <c r="G43">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -2081,7 +2162,9 @@
         <v>9</v>
       </c>
       <c r="F44" s="3"/>
-      <c r="G44"/>
+      <c r="G44">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -2102,7 +2185,9 @@
       <c r="F45" t="s">
         <v>3</v>
       </c>
-      <c r="G45"/>
+      <c r="G45">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -2123,7 +2208,9 @@
       <c r="F46" t="s">
         <v>3</v>
       </c>
-      <c r="G46"/>
+      <c r="G46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -2144,6 +2231,9 @@
       <c r="F47" t="s">
         <v>3</v>
       </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -2161,8 +2251,11 @@
       <c r="E48" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2178,8 +2271,11 @@
       <c r="E49" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2195,8 +2291,11 @@
       <c r="E50" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2212,8 +2311,11 @@
       <c r="E51" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2229,8 +2331,11 @@
       <c r="E52" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2246,8 +2351,11 @@
       <c r="E53" s="3" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2264,8 +2372,11 @@
         <v>226</v>
       </c>
       <c r="F54" s="3"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2282,8 +2393,11 @@
         <v>226</v>
       </c>
       <c r="F55" s="3"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2299,8 +2413,11 @@
       <c r="E56" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2316,8 +2433,11 @@
       <c r="E57" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2333,8 +2453,11 @@
       <c r="E58" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2351,8 +2474,11 @@
         <v>12</v>
       </c>
       <c r="F59" s="3"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2368,8 +2494,11 @@
       <c r="E60" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2385,8 +2514,11 @@
       <c r="E61" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>68</v>
       </c>
@@ -2403,8 +2535,11 @@
         <v>1</v>
       </c>
       <c r="F62" s="3"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -2420,8 +2555,11 @@
       <c r="E63" s="3" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2437,8 +2575,11 @@
       <c r="E64" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -2455,8 +2596,11 @@
         <v>12</v>
       </c>
       <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -2472,8 +2616,11 @@
       <c r="E66" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>139</v>
       </c>
@@ -2489,8 +2636,11 @@
       <c r="E67" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -2507,8 +2657,11 @@
         <v>227</v>
       </c>
       <c r="F68" s="3"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>75</v>
       </c>
@@ -2525,8 +2678,11 @@
         <v>1</v>
       </c>
       <c r="F69" s="3"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -2542,8 +2698,11 @@
       <c r="E70" s="3" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>77</v>
       </c>
@@ -2559,8 +2718,11 @@
       <c r="E71" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>78</v>
       </c>
@@ -2576,8 +2738,11 @@
       <c r="E72" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -2594,8 +2759,11 @@
         <v>9</v>
       </c>
       <c r="F73" s="3"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>80</v>
       </c>
@@ -2612,8 +2780,11 @@
         <v>9</v>
       </c>
       <c r="F74" s="3"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>81</v>
       </c>
@@ -2630,8 +2801,11 @@
         <v>1</v>
       </c>
       <c r="F75" s="3"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -2648,8 +2822,11 @@
         <v>226</v>
       </c>
       <c r="F76" s="3"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -2666,8 +2843,11 @@
         <v>9</v>
       </c>
       <c r="F77" s="3"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -2684,8 +2864,11 @@
         <v>9</v>
       </c>
       <c r="F78" s="3"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -2702,8 +2885,11 @@
         <v>9</v>
       </c>
       <c r="F79" s="3"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -2720,8 +2906,11 @@
         <v>226</v>
       </c>
       <c r="F80" s="3"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -2738,8 +2927,11 @@
         <v>9</v>
       </c>
       <c r="F81" s="3"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2755,8 +2947,11 @@
       <c r="E82" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -2773,8 +2968,11 @@
         <v>9</v>
       </c>
       <c r="F83" s="3"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2791,8 +2989,11 @@
         <v>9</v>
       </c>
       <c r="F84" s="3"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -2809,8 +3010,11 @@
         <v>9</v>
       </c>
       <c r="F85" s="3"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -2827,8 +3031,11 @@
         <v>230</v>
       </c>
       <c r="F86" s="3"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -2845,8 +3052,11 @@
         <v>227</v>
       </c>
       <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>94</v>
       </c>
@@ -2863,8 +3073,11 @@
         <v>1</v>
       </c>
       <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>95</v>
       </c>
@@ -2881,8 +3094,11 @@
         <v>1</v>
       </c>
       <c r="F89" s="3"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>96</v>
       </c>
@@ -2899,8 +3115,11 @@
         <v>9</v>
       </c>
       <c r="F90" s="3"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>97</v>
       </c>
@@ -2917,8 +3136,11 @@
         <v>9</v>
       </c>
       <c r="F91" s="3"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>140</v>
       </c>
@@ -2935,8 +3157,11 @@
         <v>9</v>
       </c>
       <c r="F92" s="3"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -2955,8 +3180,11 @@
       <c r="F93" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -2975,8 +3203,11 @@
       <c r="F94" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -2995,8 +3226,11 @@
       <c r="F95" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -3011,6 +3245,9 @@
       </c>
       <c r="E96" s="3" t="s">
         <v>226</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -3029,6 +3266,9 @@
       <c r="E97" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
@@ -3047,6 +3287,9 @@
         <v>9</v>
       </c>
       <c r="F98" s="3"/>
+      <c r="G98">
+        <v>1</v>
+      </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
@@ -3064,6 +3307,9 @@
       <c r="E99" s="3" t="s">
         <v>226</v>
       </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
@@ -3082,6 +3328,9 @@
         <v>1</v>
       </c>
       <c r="F100" s="3"/>
+      <c r="G100">
+        <v>1</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
@@ -3100,6 +3349,9 @@
         <v>226</v>
       </c>
       <c r="F101" s="3"/>
+      <c r="G101">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
@@ -3118,6 +3370,9 @@
         <v>226</v>
       </c>
       <c r="F102" s="3"/>
+      <c r="G102">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
@@ -3136,6 +3391,9 @@
         <v>227</v>
       </c>
       <c r="F103" s="3"/>
+      <c r="G103">
+        <v>1</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
@@ -3154,6 +3412,9 @@
         <v>9</v>
       </c>
       <c r="F104" s="3"/>
+      <c r="G104">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
@@ -3193,6 +3454,9 @@
         <v>226</v>
       </c>
       <c r="F106" s="3"/>
+      <c r="G106">
+        <v>1</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
@@ -3211,6 +3475,9 @@
         <v>9</v>
       </c>
       <c r="F107" s="3"/>
+      <c r="G107">
+        <v>1</v>
+      </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
@@ -3229,6 +3496,9 @@
         <v>1</v>
       </c>
       <c r="F108" s="3"/>
+      <c r="G108">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
@@ -3247,6 +3517,9 @@
         <v>226</v>
       </c>
       <c r="F109" s="3"/>
+      <c r="G109">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
@@ -3265,6 +3538,9 @@
         <v>9</v>
       </c>
       <c r="F110" s="3"/>
+      <c r="G110">
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -3283,6 +3559,9 @@
         <v>9</v>
       </c>
       <c r="F111" s="3"/>
+      <c r="G111">
+        <v>1</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
@@ -3301,8 +3580,11 @@
         <v>1</v>
       </c>
       <c r="F112" s="3"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>141</v>
       </c>
@@ -3319,8 +3601,11 @@
         <v>9</v>
       </c>
       <c r="F113" s="3"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>142</v>
       </c>
@@ -3336,8 +3621,11 @@
       <c r="E114" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>145</v>
       </c>
@@ -3353,8 +3641,11 @@
       <c r="E115" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>147</v>
       </c>
@@ -3370,8 +3661,11 @@
       <c r="E116" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>149</v>
       </c>
@@ -3387,8 +3681,11 @@
       <c r="E117" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>151</v>
       </c>
@@ -3404,8 +3701,11 @@
       <c r="E118" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>153</v>
       </c>
@@ -3421,8 +3721,11 @@
       <c r="E119" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>155</v>
       </c>
@@ -3438,8 +3741,11 @@
       <c r="E120" s="3" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>156</v>
       </c>
@@ -3455,8 +3761,11 @@
       <c r="E121" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>177</v>
       </c>
@@ -3472,8 +3781,11 @@
       <c r="E122" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>178</v>
       </c>
@@ -3489,8 +3801,11 @@
       <c r="E123" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>179</v>
       </c>
@@ -3506,8 +3821,11 @@
       <c r="E124" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>180</v>
       </c>
@@ -3523,8 +3841,11 @@
       <c r="E125" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>181</v>
       </c>
@@ -3540,8 +3861,11 @@
       <c r="E126" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>182</v>
       </c>
@@ -3557,8 +3881,11 @@
       <c r="E127" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>183</v>
       </c>
@@ -3574,8 +3901,11 @@
       <c r="E128" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>184</v>
       </c>
@@ -3591,8 +3921,11 @@
       <c r="E129" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>185</v>
       </c>
@@ -3608,8 +3941,11 @@
       <c r="E130" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>186</v>
       </c>
@@ -3625,8 +3961,11 @@
       <c r="E131" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>187</v>
       </c>
@@ -3642,8 +3981,11 @@
       <c r="E132" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>188</v>
       </c>
@@ -3659,8 +4001,11 @@
       <c r="E133" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>189</v>
       </c>
@@ -3676,8 +4021,11 @@
       <c r="E134" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>190</v>
       </c>
@@ -3696,8 +4044,11 @@
       <c r="F135" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>191</v>
       </c>
@@ -3713,8 +4064,11 @@
       <c r="E136" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>192</v>
       </c>
@@ -3730,8 +4084,11 @@
       <c r="E137" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>159</v>
       </c>
@@ -3750,8 +4107,11 @@
       <c r="F138" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>160</v>
       </c>
@@ -3767,8 +4127,11 @@
       <c r="E139" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>161</v>
       </c>
@@ -3784,8 +4147,11 @@
       <c r="E140" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>162</v>
       </c>
@@ -3801,8 +4167,11 @@
       <c r="E141" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>163</v>
       </c>
@@ -3818,8 +4187,11 @@
       <c r="E142" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>164</v>
       </c>
@@ -3835,8 +4207,11 @@
       <c r="E143" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>165</v>
       </c>
@@ -3852,8 +4227,11 @@
       <c r="E144" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>166</v>
       </c>
@@ -3869,8 +4247,11 @@
       <c r="E145" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>167</v>
       </c>
@@ -3886,8 +4267,11 @@
       <c r="E146" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>168</v>
       </c>
@@ -3903,8 +4287,11 @@
       <c r="E147" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>169</v>
       </c>
@@ -3920,8 +4307,11 @@
       <c r="E148" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>170</v>
       </c>
@@ -3937,8 +4327,11 @@
       <c r="E149" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>171</v>
       </c>
@@ -3954,8 +4347,11 @@
       <c r="E150" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>172</v>
       </c>
@@ -3971,8 +4367,11 @@
       <c r="E151" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>173</v>
       </c>
@@ -3988,8 +4387,11 @@
       <c r="E152" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>174</v>
       </c>
@@ -4005,8 +4407,11 @@
       <c r="E153" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>175</v>
       </c>
@@ -4022,8 +4427,11 @@
       <c r="E154" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>120</v>
       </c>
@@ -4039,8 +4447,11 @@
       <c r="E155" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>121</v>
       </c>
@@ -4056,8 +4467,11 @@
       <c r="E156" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>122</v>
       </c>
@@ -4073,8 +4487,11 @@
       <c r="E157" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>123</v>
       </c>
@@ -4090,8 +4507,11 @@
       <c r="E158" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>124</v>
       </c>
@@ -4107,8 +4527,11 @@
       <c r="E159" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>125</v>
       </c>
@@ -4124,8 +4547,11 @@
       <c r="E160" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>126</v>
       </c>
@@ -4144,8 +4570,11 @@
       <c r="F161" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>127</v>
       </c>
@@ -4161,8 +4590,11 @@
       <c r="E162" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>128</v>
       </c>
@@ -4178,8 +4610,11 @@
       <c r="E163" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>129</v>
       </c>
@@ -4195,8 +4630,11 @@
       <c r="E164" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>130</v>
       </c>
@@ -4212,8 +4650,11 @@
       <c r="E165" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>131</v>
       </c>
@@ -4229,8 +4670,11 @@
       <c r="E166" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>132</v>
       </c>
@@ -4246,8 +4690,11 @@
       <c r="E167" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>134</v>
       </c>
@@ -4263,8 +4710,11 @@
       <c r="E168" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>133</v>
       </c>
@@ -4280,8 +4730,11 @@
       <c r="E169" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>135</v>
       </c>
@@ -4297,23 +4750,26 @@
       <c r="E170" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C171" s="21"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C172" s="21"/>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C173" s="21"/>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C174" s="21"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C175" s="21"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C176" s="21"/>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.2">
@@ -4361,8 +4817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB22EBC-98B5-0A4B-BE66-A269A8B9C2CC}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4438,8 +4894,6 @@
       <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -4460,8 +4914,6 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -4482,8 +4934,6 @@
       <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -4504,8 +4954,6 @@
       <c r="F6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -4526,8 +4974,6 @@
       <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">

</xml_diff>